<commit_message>
edited .xlxs /w plots
</commit_message>
<xml_diff>
--- a/zadanie6/data/zadanie6_119229_119233.xlsx
+++ b/zadanie6/data/zadanie6_119229_119233.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiii5\Desktop\Notatki_stacja\UKSW\MAGISTERKA\Algorytmy inspirowane natura\algorytmy_inspirowane_natura\zadanie6\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AACFE4D3-086A-43F8-AF38-DCE25EA08B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA08074-BF19-4172-A155-98C46E229409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{AC4D1C06-2117-431D-8297-911A5AE3D37B}"/>
   </bookViews>
@@ -170,7 +170,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6610,7 +6610,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13865,36 +13865,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Kung!$A$2:$A$4</c:f>
+              <c:f>Kung!$A$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.731298</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.831682</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3648009999999999</c:v>
+                  <c:v>-2.455905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kung!$B$2:$B$4</c:f>
+              <c:f>Kung!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.4346190000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.1686809999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.872058</c:v>
+                  <c:v>-4.228561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13936,48 +13924,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Kung!$D$2:$D$6</c:f>
+              <c:f>Kung!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.6013250000000001</c:v>
+                  <c:v>-2.1665160000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.691554</c:v>
+                  <c:v>-2.1271</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8188610000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.855391</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8605419999999999</c:v>
+                  <c:v>-2.107739</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kung!$E$2:$E$6</c:f>
+              <c:f>Kung!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.989976</c:v>
+                  <c:v>-2.409151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9262679999999999</c:v>
+                  <c:v>-3.4599340000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5870150000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.450393</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2395049999999999</c:v>
+                  <c:v>-3.806092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14019,48 +13995,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Kung!$G$2:$G$6</c:f>
+              <c:f>Kung!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.4793149999999999</c:v>
+                  <c:v>-2.1182240000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.481762</c:v>
+                  <c:v>-1.903939</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.700906</c:v>
+                  <c:v>-1.8928339999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7731619999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8424229999999999</c:v>
+                  <c:v>-1.8466959999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kung!$H$2:$H$6</c:f>
+              <c:f>Kung!$H$2:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.8987980000000002</c:v>
+                  <c:v>-2.425516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6432709999999999</c:v>
+                  <c:v>-2.734194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5627949999999999</c:v>
+                  <c:v>-2.9947249999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1283080000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.0882719999999999</c:v>
+                  <c:v>-3.1946539999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14102,60 +14072,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Kung!$J$2:$J$8</c:f>
+              <c:f>Kung!$J$2:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.4406300000000001</c:v>
+                  <c:v>-1.762203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.448885</c:v>
+                  <c:v>-1.759061</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.451187</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.528302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.700102</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7654540000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8268979999999999</c:v>
+                  <c:v>-1.707773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kung!$K$2:$K$8</c:f>
+              <c:f>Kung!$K$2:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.8518569999999999</c:v>
+                  <c:v>-2.169295</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7662300000000002</c:v>
+                  <c:v>-2.78329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.730248</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5239639999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4015520000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.0750109999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4619660000000001</c:v>
+                  <c:v>-3.1941060000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14197,42 +14143,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Kung!$M$2:$M$5</c:f>
+              <c:f>Kung!$M$2:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.3686659999999999</c:v>
+                  <c:v>-1.7261120000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5923020000000001</c:v>
+                  <c:v>-1.6806319999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6817279999999999</c:v>
+                  <c:v>-1.672083</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7588429999999999</c:v>
+                  <c:v>-1.65422</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.629599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.3771770000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kung!$N$2:$N$5</c:f>
+              <c:f>Kung!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.847254</c:v>
+                  <c:v>-1.6472819999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.175103</c:v>
+                  <c:v>-2.2279979999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9501520000000001</c:v>
+                  <c:v>-2.7527149999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7438670000000001</c:v>
+                  <c:v>-2.9016470000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.9389810000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.0617939999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17284,7 +17242,7 @@
   <dimension ref="A1:B1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25308,7 +25266,7 @@
   <dimension ref="A1:B1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33332,7 +33290,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33491,10 +33449,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6976EDF-AE0F-4770-9EEC-146DBC59C342}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33533,160 +33491,116 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.731298</v>
+        <v>-2.455905</v>
       </c>
       <c r="B2">
-        <v>3.4346190000000001</v>
+        <v>-4.228561</v>
       </c>
       <c r="D2">
-        <v>1.6013250000000001</v>
+        <v>-2.1665160000000001</v>
       </c>
       <c r="E2">
-        <v>2.989976</v>
+        <v>-2.409151</v>
       </c>
       <c r="G2">
-        <v>1.4793149999999999</v>
+        <v>-2.1182240000000001</v>
       </c>
       <c r="H2">
-        <v>2.8987980000000002</v>
+        <v>-2.425516</v>
       </c>
       <c r="J2">
-        <v>1.4406300000000001</v>
+        <v>-1.762203</v>
       </c>
       <c r="K2">
-        <v>2.8518569999999999</v>
+        <v>-2.169295</v>
       </c>
       <c r="M2">
-        <v>1.3686659999999999</v>
+        <v>-1.7261120000000001</v>
       </c>
       <c r="N2">
-        <v>2.847254</v>
+        <v>-1.6472819999999999</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.831682</v>
-      </c>
-      <c r="B3">
-        <v>3.1686809999999999</v>
-      </c>
       <c r="D3">
-        <v>1.691554</v>
+        <v>-2.1271</v>
       </c>
       <c r="E3">
-        <v>2.9262679999999999</v>
+        <v>-3.4599340000000001</v>
       </c>
       <c r="G3">
-        <v>1.481762</v>
+        <v>-1.903939</v>
       </c>
       <c r="H3">
-        <v>2.6432709999999999</v>
+        <v>-2.734194</v>
       </c>
       <c r="J3">
-        <v>1.448885</v>
+        <v>-1.759061</v>
       </c>
       <c r="K3">
-        <v>2.7662300000000002</v>
+        <v>-2.78329</v>
       </c>
       <c r="M3">
-        <v>1.5923020000000001</v>
+        <v>-1.6806319999999999</v>
       </c>
       <c r="N3">
-        <v>2.175103</v>
+        <v>-2.2279979999999999</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2.3648009999999999</v>
-      </c>
-      <c r="B4">
-        <v>2.872058</v>
-      </c>
       <c r="D4">
-        <v>1.8188610000000001</v>
+        <v>-2.107739</v>
       </c>
       <c r="E4">
-        <v>2.5870150000000001</v>
+        <v>-3.806092</v>
       </c>
       <c r="G4">
-        <v>1.700906</v>
+        <v>-1.8928339999999999</v>
       </c>
       <c r="H4">
-        <v>2.5627949999999999</v>
+        <v>-2.9947249999999999</v>
       </c>
       <c r="J4">
-        <v>1.451187</v>
+        <v>-1.707773</v>
       </c>
       <c r="K4">
-        <v>2.730248</v>
+        <v>-3.1941060000000001</v>
       </c>
       <c r="M4">
-        <v>1.6817279999999999</v>
+        <v>-1.672083</v>
       </c>
       <c r="N4">
-        <v>1.9501520000000001</v>
+        <v>-2.7527149999999998</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>1.855391</v>
-      </c>
-      <c r="E5">
-        <v>2.450393</v>
-      </c>
       <c r="G5">
-        <v>1.7731619999999999</v>
+        <v>-1.8466959999999999</v>
       </c>
       <c r="H5">
-        <v>2.1283080000000001</v>
-      </c>
-      <c r="J5">
-        <v>1.528302</v>
-      </c>
-      <c r="K5">
-        <v>2.5239639999999999</v>
+        <v>-3.1946539999999999</v>
       </c>
       <c r="M5">
-        <v>1.7588429999999999</v>
+        <v>-1.65422</v>
       </c>
       <c r="N5">
-        <v>1.7438670000000001</v>
+        <v>-2.9016470000000001</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>1.8605419999999999</v>
-      </c>
-      <c r="E6">
-        <v>2.2395049999999999</v>
-      </c>
-      <c r="G6">
-        <v>1.8424229999999999</v>
-      </c>
-      <c r="H6">
-        <v>2.0882719999999999</v>
-      </c>
-      <c r="J6">
-        <v>1.700102</v>
-      </c>
-      <c r="K6">
-        <v>2.4015520000000001</v>
+      <c r="M6">
+        <v>-1.629599</v>
+      </c>
+      <c r="N6">
+        <v>-2.9389810000000001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J7">
-        <v>1.7654540000000001</v>
-      </c>
-      <c r="K7">
-        <v>2.0750109999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J8">
-        <v>1.8268979999999999</v>
-      </c>
-      <c r="K8">
-        <v>1.4619660000000001</v>
+      <c r="M7">
+        <v>-1.3771770000000001</v>
+      </c>
+      <c r="N7">
+        <v>-3.0617939999999999</v>
       </c>
     </row>
   </sheetData>
@@ -33696,6 +33610,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a663b722-cd90-4b46-bde6-5b0d51e253ee" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003A2448C643F3684794B5EAB11DBF7E98" ma:contentTypeVersion="11" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="a38f60718af649234f0e5850c57c1c5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a663b722-cd90-4b46-bde6-5b0d51e253ee" xmlns:ns4="40925ba0-53c2-4345-973a-5522edab24fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f09511bafd80d759577239a96edd252" ns3:_="" ns4:_="">
     <xsd:import namespace="a663b722-cd90-4b46-bde6-5b0d51e253ee"/>
@@ -33904,24 +33835,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A66CF619-8317-4177-BFA9-A246C96E8AEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40925ba0-53c2-4345-973a-5522edab24fe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a663b722-cd90-4b46-bde6-5b0d51e253ee"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a663b722-cd90-4b46-bde6-5b0d51e253ee" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA704B76-9DF8-4463-9590-E45B12395842}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7BA45A-3992-4150-A760-34E0B0C09C0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33938,29 +33877,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA704B76-9DF8-4463-9590-E45B12395842}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A66CF619-8317-4177-BFA9-A246C96E8AEC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40925ba0-53c2-4345-973a-5522edab24fe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a663b722-cd90-4b46-bde6-5b0d51e253ee"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>